<commit_message>
fecho janeiro, agora e que e
</commit_message>
<xml_diff>
--- a/GestorReceitas/Janeiro/relatorioMensal_backup_janeiro_20250204_232137.xlsx
+++ b/GestorReceitas/Janeiro/relatorioMensal_backup_janeiro_20250204_232137.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pessoal\AssociacaodePais\School\GestorReceitas\Janeiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A740A84-B85A-4758-9CC5-0FBD3B7D0D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BCBAB6-3523-4FA4-A5E4-0B4511B4637E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="453">
   <si>
     <t>Nome</t>
   </si>
@@ -1383,6 +1383,18 @@
   </si>
   <si>
     <t>Quota</t>
+  </si>
+  <si>
+    <t>Confirmar Karate</t>
+  </si>
+  <si>
+    <t>Pagou em fevereiro</t>
+  </si>
+  <si>
+    <t>Telefonar</t>
+  </si>
+  <si>
+    <t>falta carnaval</t>
   </si>
 </sst>
 </file>
@@ -1535,36 +1547,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="150">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
+  <dxfs count="146">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -2597,8 +2580,8 @@
   <dimension ref="A1:U146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,7 +2590,7 @@
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="17" width="12.28515625" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2667,7 +2650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -2718,15 +2701,10 @@
       <c r="R2" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="4">
-        <v>0</v>
-      </c>
-      <c r="T2" s="4">
-        <f>O2-S2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
@@ -2777,13 +2755,8 @@
       <c r="R3" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="4">
-        <v>0</v>
-      </c>
-      <c r="T3" s="4">
-        <f t="shared" ref="T3:T66" si="1">O3-S3</f>
-        <v>0</v>
-      </c>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -2838,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="T3:T25" si="1">O4-S4</f>
         <v>0</v>
       </c>
     </row>
@@ -2899,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>32</v>
       </c>
@@ -2950,19 +2923,14 @@
       <c r="R6" t="s">
         <v>35</v>
       </c>
-      <c r="S6" s="4">
-        <v>0</v>
-      </c>
-      <c r="T6" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+    </row>
+    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C7">
@@ -3006,18 +2974,14 @@
         <f t="shared" si="0"/>
         <v>-44</v>
       </c>
+      <c r="Q7" s="4"/>
       <c r="R7" t="s">
         <v>38</v>
       </c>
-      <c r="S7" s="4">
-        <v>0</v>
-      </c>
-      <c r="T7" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+    </row>
+    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>39</v>
       </c>
@@ -3069,13 +3033,8 @@
       <c r="R8" t="s">
         <v>41</v>
       </c>
-      <c r="S8" s="4">
-        <v>0</v>
-      </c>
-      <c r="T8" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
     </row>
     <row r="9" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
@@ -3134,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -3185,13 +3144,8 @@
       <c r="R10" t="s">
         <v>49</v>
       </c>
-      <c r="S10" s="4">
-        <v>0</v>
-      </c>
-      <c r="T10" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
     </row>
     <row r="11" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -3251,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>54</v>
       </c>
@@ -3305,15 +3259,10 @@
       <c r="R12" t="s">
         <v>56</v>
       </c>
-      <c r="S12" s="4">
-        <v>0</v>
-      </c>
-      <c r="T12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+    </row>
+    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>57</v>
       </c>
@@ -3364,15 +3313,10 @@
       <c r="R13" t="s">
         <v>59</v>
       </c>
-      <c r="S13" s="4">
-        <v>0</v>
-      </c>
-      <c r="T13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+    </row>
+    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>60</v>
       </c>
@@ -3424,15 +3368,10 @@
       <c r="R14" t="s">
         <v>41</v>
       </c>
-      <c r="S14" s="4">
-        <v>0</v>
-      </c>
-      <c r="T14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+    </row>
+    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>62</v>
       </c>
@@ -3483,15 +3422,10 @@
       <c r="R15" t="s">
         <v>64</v>
       </c>
-      <c r="S15" s="4">
-        <v>0</v>
-      </c>
-      <c r="T15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+    </row>
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>65</v>
       </c>
@@ -3542,13 +3476,8 @@
       <c r="R16" t="s">
         <v>67</v>
       </c>
-      <c r="S16" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="T16" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
     </row>
     <row r="17" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -3667,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>73</v>
       </c>
@@ -3719,13 +3648,8 @@
       <c r="R19" t="s">
         <v>75</v>
       </c>
-      <c r="S19" s="4">
-        <v>0</v>
-      </c>
-      <c r="T19" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
     </row>
     <row r="20" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
@@ -3842,7 +3766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>82</v>
       </c>
@@ -3893,13 +3817,8 @@
       <c r="R22" t="s">
         <v>84</v>
       </c>
-      <c r="S22" s="4">
-        <v>0</v>
-      </c>
-      <c r="T22" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
     </row>
     <row r="23" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
@@ -3958,7 +3877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>88</v>
       </c>
@@ -4004,15 +3923,10 @@
       <c r="R24" t="s">
         <v>90</v>
       </c>
-      <c r="S24" s="4">
-        <v>-45</v>
-      </c>
-      <c r="T24" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+    </row>
+    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>91</v>
       </c>
@@ -4065,10 +3979,7 @@
       <c r="R25" t="s">
         <v>93</v>
       </c>
-      <c r="T25" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="T25" s="4"/>
     </row>
     <row r="26" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
@@ -4174,7 +4085,7 @@
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
     </row>
-    <row r="28" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>100</v>
       </c>
@@ -4385,7 +4296,7 @@
       <c r="S31" s="4"/>
       <c r="T31" s="4"/>
     </row>
-    <row r="32" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>112</v>
       </c>
@@ -4439,7 +4350,7 @@
       <c r="S32" s="4"/>
       <c r="T32" s="4"/>
     </row>
-    <row r="33" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>115</v>
       </c>
@@ -4493,11 +4404,11 @@
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
     </row>
-    <row r="34" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C34">
@@ -4597,11 +4508,11 @@
       <c r="S35" s="4"/>
       <c r="T35" s="4"/>
     </row>
-    <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C36">
@@ -4914,7 +4825,7 @@
       <c r="S41" s="4"/>
       <c r="T41" s="4"/>
     </row>
-    <row r="42" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>141</v>
       </c>
@@ -4968,7 +4879,7 @@
       <c r="S42" s="4"/>
       <c r="T42" s="4"/>
     </row>
-    <row r="43" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>144</v>
       </c>
@@ -5022,7 +4933,7 @@
       <c r="S43" s="4"/>
       <c r="T43" s="4"/>
     </row>
-    <row r="44" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>147</v>
       </c>
@@ -5076,7 +4987,7 @@
       <c r="S44" s="4"/>
       <c r="T44" s="4"/>
     </row>
-    <row r="45" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>150</v>
       </c>
@@ -5131,7 +5042,7 @@
       <c r="S45" s="4"/>
       <c r="T45" s="4"/>
     </row>
-    <row r="46" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>153</v>
       </c>
@@ -5237,7 +5148,7 @@
       <c r="S47" s="4"/>
       <c r="T47" s="4"/>
     </row>
-    <row r="48" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>159</v>
       </c>
@@ -5344,11 +5255,11 @@
       <c r="T49" s="4"/>
       <c r="U49" s="5"/>
     </row>
-    <row r="50" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C50">
@@ -5392,17 +5303,18 @@
         <f t="shared" si="0"/>
         <v>-37.5</v>
       </c>
+      <c r="Q50" s="4"/>
       <c r="R50" t="s">
         <v>167</v>
       </c>
       <c r="S50" s="4"/>
       <c r="T50" s="4"/>
     </row>
-    <row r="51" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C51">
@@ -5453,7 +5365,7 @@
       <c r="T51" s="4"/>
       <c r="U51" s="5"/>
     </row>
-    <row r="52" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>171</v>
       </c>
@@ -5505,7 +5417,9 @@
       <c r="R52" t="s">
         <v>173</v>
       </c>
-      <c r="S52" s="4"/>
+      <c r="S52" s="4" t="s">
+        <v>449</v>
+      </c>
       <c r="T52" s="4"/>
     </row>
     <row r="53" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -5560,7 +5474,7 @@
       <c r="S53" s="4"/>
       <c r="T53" s="4"/>
     </row>
-    <row r="54" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>177</v>
       </c>
@@ -5716,7 +5630,7 @@
       <c r="S56" s="4"/>
       <c r="T56" s="4"/>
     </row>
-    <row r="57" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>186</v>
       </c>
@@ -5874,7 +5788,7 @@
       <c r="S59" s="4"/>
       <c r="T59" s="4"/>
     </row>
-    <row r="60" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>195</v>
       </c>
@@ -5928,11 +5842,11 @@
       <c r="S60" s="4"/>
       <c r="T60" s="4"/>
     </row>
-    <row r="61" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C61">
@@ -5976,17 +5890,18 @@
         <f t="shared" si="0"/>
         <v>-38</v>
       </c>
+      <c r="Q61" s="4"/>
       <c r="R61" t="s">
         <v>200</v>
       </c>
       <c r="S61" s="4"/>
       <c r="T61" s="4"/>
     </row>
-    <row r="62" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C62">
@@ -6034,11 +5949,11 @@
       <c r="S62" s="4"/>
       <c r="T62" s="4"/>
     </row>
-    <row r="63" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C63">
@@ -6083,17 +5998,20 @@
         <f t="shared" si="0"/>
         <v>-27</v>
       </c>
+      <c r="Q63" s="4"/>
       <c r="R63" t="s">
         <v>206</v>
       </c>
-      <c r="S63" s="4"/>
+      <c r="S63" s="4" t="s">
+        <v>450</v>
+      </c>
       <c r="T63" s="4"/>
     </row>
-    <row r="64" spans="1:21" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C64">
@@ -6137,13 +6055,14 @@
         <f t="shared" si="0"/>
         <v>-23</v>
       </c>
+      <c r="Q64" s="4"/>
       <c r="R64" t="s">
         <v>209</v>
       </c>
       <c r="S64" s="4"/>
       <c r="T64" s="4"/>
     </row>
-    <row r="65" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>210</v>
       </c>
@@ -6249,7 +6168,7 @@
       <c r="S66" s="4"/>
       <c r="T66" s="4"/>
     </row>
-    <row r="67" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>215</v>
       </c>
@@ -6303,7 +6222,7 @@
       <c r="S67" s="4"/>
       <c r="T67" s="4"/>
     </row>
-    <row r="68" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>218</v>
       </c>
@@ -6357,7 +6276,7 @@
       <c r="S68" s="4"/>
       <c r="T68" s="4"/>
     </row>
-    <row r="69" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>221</v>
       </c>
@@ -6412,11 +6331,11 @@
       <c r="S69" s="4"/>
       <c r="T69" s="4"/>
     </row>
-    <row r="70" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C70">
@@ -6441,7 +6360,7 @@
         <v>23</v>
       </c>
       <c r="J70" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K70" s="2"/>
       <c r="L70" s="2">
@@ -6458,15 +6377,16 @@
       </c>
       <c r="P70" s="3">
         <f t="shared" si="2"/>
-        <v>-26</v>
-      </c>
+        <v>-14</v>
+      </c>
+      <c r="Q70" s="4"/>
       <c r="R70" t="s">
         <v>226</v>
       </c>
       <c r="S70" s="4"/>
       <c r="T70" s="4"/>
     </row>
-    <row r="71" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>227</v>
       </c>
@@ -6517,14 +6437,16 @@
       <c r="R71" t="s">
         <v>229</v>
       </c>
-      <c r="S71" s="4"/>
+      <c r="S71" s="4" t="s">
+        <v>452</v>
+      </c>
       <c r="T71" s="4"/>
     </row>
-    <row r="72" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C72">
@@ -6568,13 +6490,14 @@
         <f t="shared" si="2"/>
         <v>-68</v>
       </c>
+      <c r="Q72" s="4"/>
       <c r="R72" t="s">
         <v>232</v>
       </c>
       <c r="S72" s="4"/>
       <c r="T72" s="4"/>
     </row>
-    <row r="73" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>233</v>
       </c>
@@ -6681,11 +6604,11 @@
       <c r="S74" s="4"/>
       <c r="T74" s="4"/>
     </row>
-    <row r="75" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" ht="15" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C75">
@@ -6734,7 +6657,7 @@
       <c r="S75" s="4"/>
       <c r="T75" s="4"/>
     </row>
-    <row r="76" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="15" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
         <v>242</v>
       </c>
@@ -6786,7 +6709,7 @@
       <c r="S76" s="4"/>
       <c r="T76" s="4"/>
     </row>
-    <row r="77" spans="1:20" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>244</v>
       </c>
@@ -6845,7 +6768,7 @@
       <c r="A78" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C78">
@@ -6878,14 +6801,15 @@
         <v>0</v>
       </c>
       <c r="N78" s="2">
-        <v>62.5</v>
+        <f>62.5-62.5</f>
+        <v>0</v>
       </c>
       <c r="O78" s="3">
         <v>0</v>
       </c>
       <c r="P78" s="3">
         <f t="shared" si="2"/>
-        <v>13.5</v>
+        <v>-49</v>
       </c>
       <c r="R78" t="s">
         <v>125</v>
@@ -6893,7 +6817,7 @@
       <c r="S78" s="4"/>
       <c r="T78" s="4"/>
     </row>
-    <row r="79" spans="1:20" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>249</v>
       </c>
@@ -6942,14 +6866,16 @@
       <c r="R79" t="s">
         <v>251</v>
       </c>
-      <c r="S79" s="4"/>
+      <c r="S79" s="4" t="s">
+        <v>449</v>
+      </c>
       <c r="T79" s="4"/>
     </row>
-    <row r="80" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C80">
@@ -6993,13 +6919,14 @@
         <f t="shared" si="2"/>
         <v>-22.5</v>
       </c>
+      <c r="Q80" s="4"/>
       <c r="R80" t="s">
         <v>254</v>
       </c>
       <c r="S80" s="4"/>
       <c r="T80" s="4"/>
     </row>
-    <row r="81" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>255</v>
       </c>
@@ -7053,7 +6980,7 @@
       <c r="S81" s="4"/>
       <c r="T81" s="4"/>
     </row>
-    <row r="82" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>258</v>
       </c>
@@ -7107,7 +7034,7 @@
       <c r="S82" s="4"/>
       <c r="T82" s="4"/>
     </row>
-    <row r="83" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>261</v>
       </c>
@@ -7156,10 +7083,12 @@
       <c r="R83" t="s">
         <v>263</v>
       </c>
-      <c r="S83" s="4"/>
+      <c r="S83" s="4" t="s">
+        <v>450</v>
+      </c>
       <c r="T83" s="4"/>
     </row>
-    <row r="84" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>264</v>
       </c>
@@ -7214,7 +7143,7 @@
       <c r="S84" s="4"/>
       <c r="T84" s="4"/>
     </row>
-    <row r="85" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>267</v>
       </c>
@@ -7269,7 +7198,7 @@
       <c r="S85" s="4"/>
       <c r="T85" s="4"/>
     </row>
-    <row r="86" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>269</v>
       </c>
@@ -7321,7 +7250,7 @@
       <c r="S86" s="4"/>
       <c r="T86" s="4"/>
     </row>
-    <row r="87" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>272</v>
       </c>
@@ -7375,7 +7304,7 @@
       <c r="S87" s="4"/>
       <c r="T87" s="4"/>
     </row>
-    <row r="88" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>275</v>
       </c>
@@ -7430,7 +7359,7 @@
       <c r="S88" s="4"/>
       <c r="T88" s="4"/>
     </row>
-    <row r="89" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>277</v>
       </c>
@@ -7536,7 +7465,7 @@
       <c r="S90" s="4"/>
       <c r="T90" s="4"/>
     </row>
-    <row r="91" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>283</v>
       </c>
@@ -7587,10 +7516,12 @@
       <c r="R91" t="s">
         <v>285</v>
       </c>
-      <c r="S91" s="4"/>
+      <c r="S91" s="4" t="s">
+        <v>451</v>
+      </c>
       <c r="T91" s="4"/>
     </row>
-    <row r="92" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>286</v>
       </c>
@@ -7644,11 +7575,11 @@
       <c r="S92" s="4"/>
       <c r="T92" s="4"/>
     </row>
-    <row r="93" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C93">
@@ -7693,6 +7624,7 @@
         <f t="shared" si="2"/>
         <v>-19</v>
       </c>
+      <c r="Q93" s="4"/>
       <c r="R93" t="s">
         <v>291</v>
       </c>
@@ -7754,7 +7686,7 @@
       <c r="S94" s="4"/>
       <c r="T94" s="4"/>
     </row>
-    <row r="95" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>295</v>
       </c>
@@ -7809,7 +7741,7 @@
       <c r="S95" s="4"/>
       <c r="T95" s="4"/>
     </row>
-    <row r="96" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>298</v>
       </c>
@@ -7915,11 +7847,11 @@
       <c r="S97" s="4"/>
       <c r="T97" s="4"/>
     </row>
-    <row r="98" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C98">
@@ -7964,10 +7896,12 @@
       <c r="R98" t="s">
         <v>306</v>
       </c>
-      <c r="S98" s="4"/>
+      <c r="S98" s="4" t="s">
+        <v>451</v>
+      </c>
       <c r="T98" s="4"/>
     </row>
-    <row r="99" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>307</v>
       </c>
@@ -8021,11 +7955,11 @@
       <c r="S99" s="4"/>
       <c r="T99" s="4"/>
     </row>
-    <row r="100" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C100">
@@ -8069,13 +8003,16 @@
         <f t="shared" si="2"/>
         <v>-27</v>
       </c>
+      <c r="Q100" s="4"/>
       <c r="R100" t="s">
         <v>312</v>
       </c>
-      <c r="S100" s="4"/>
+      <c r="S100" s="4" t="s">
+        <v>450</v>
+      </c>
       <c r="T100" s="4"/>
     </row>
-    <row r="101" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>313</v>
       </c>
@@ -8237,7 +8174,7 @@
       <c r="S103" s="4"/>
       <c r="T103" s="4"/>
     </row>
-    <row r="104" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>322</v>
       </c>
@@ -8288,10 +8225,12 @@
       <c r="R104" t="s">
         <v>324</v>
       </c>
-      <c r="S104" s="4"/>
+      <c r="S104" s="4" t="s">
+        <v>452</v>
+      </c>
       <c r="T104" s="4"/>
     </row>
-    <row r="105" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>325</v>
       </c>
@@ -8346,11 +8285,11 @@
       <c r="S105" s="4"/>
       <c r="T105" s="4"/>
     </row>
-    <row r="106" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C106">
@@ -8394,17 +8333,18 @@
         <f t="shared" si="2"/>
         <v>-28</v>
       </c>
+      <c r="Q106" s="4"/>
       <c r="R106" t="s">
         <v>330</v>
       </c>
       <c r="S106" s="4"/>
       <c r="T106" s="4"/>
     </row>
-    <row r="107" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C107">
@@ -8448,13 +8388,14 @@
         <f t="shared" si="2"/>
         <v>-46</v>
       </c>
+      <c r="Q107" s="4"/>
       <c r="R107" t="s">
         <v>333</v>
       </c>
       <c r="S107" s="4"/>
       <c r="T107" s="4"/>
     </row>
-    <row r="108" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>334</v>
       </c>
@@ -8561,7 +8502,7 @@
       <c r="S109" s="4"/>
       <c r="T109" s="4"/>
     </row>
-    <row r="110" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>339</v>
       </c>
@@ -8615,7 +8556,7 @@
       <c r="S110" s="4"/>
       <c r="T110" s="4"/>
     </row>
-    <row r="111" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>342</v>
       </c>
@@ -8670,11 +8611,11 @@
       <c r="S111" s="4"/>
       <c r="T111" s="4"/>
     </row>
-    <row r="112" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C112">
@@ -8723,7 +8664,7 @@
       <c r="S112" s="4"/>
       <c r="T112" s="4"/>
     </row>
-    <row r="113" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>348</v>
       </c>
@@ -8777,7 +8718,7 @@
       <c r="S113" s="4"/>
       <c r="T113" s="4"/>
     </row>
-    <row r="114" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>351</v>
       </c>
@@ -8830,11 +8771,11 @@
       <c r="S114" s="4"/>
       <c r="T114" s="4"/>
     </row>
-    <row r="115" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C115">
@@ -8881,17 +8822,18 @@
         <f t="shared" si="2"/>
         <v>-27</v>
       </c>
+      <c r="Q115" s="4"/>
       <c r="R115" t="s">
         <v>356</v>
       </c>
       <c r="S115" s="4"/>
       <c r="T115" s="4"/>
     </row>
-    <row r="116" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D116" t="s">
@@ -8913,7 +8855,7 @@
         <v>23</v>
       </c>
       <c r="J116" s="2">
-        <v>12</v>
+        <v>3.5</v>
       </c>
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
@@ -8929,7 +8871,7 @@
       </c>
       <c r="P116" s="3">
         <f t="shared" si="2"/>
-        <v>-77</v>
+        <v>-68.5</v>
       </c>
       <c r="R116" t="s">
         <v>359</v>
@@ -8937,11 +8879,11 @@
       <c r="S116" s="4"/>
       <c r="T116" s="4"/>
     </row>
-    <row r="117" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C117">
@@ -8985,13 +8927,14 @@
         <f t="shared" si="2"/>
         <v>-43.5</v>
       </c>
+      <c r="Q117" s="4"/>
       <c r="R117" t="s">
         <v>362</v>
       </c>
       <c r="S117" s="4"/>
       <c r="T117" s="4"/>
     </row>
-    <row r="118" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>363</v>
       </c>
@@ -9100,8 +9043,8 @@
       <c r="S119" s="4"/>
       <c r="T119" s="4"/>
     </row>
-    <row r="120" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="6" t="s">
+    <row r="120" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
         <v>369</v>
       </c>
       <c r="B120" t="s">
@@ -9261,7 +9204,7 @@
       <c r="S122" s="4"/>
       <c r="T122" s="4"/>
     </row>
-    <row r="123" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>378</v>
       </c>
@@ -9315,7 +9258,7 @@
       <c r="S123" s="4"/>
       <c r="T123" s="4"/>
     </row>
-    <row r="124" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>381</v>
       </c>
@@ -9369,11 +9312,11 @@
       <c r="S124" s="4"/>
       <c r="T124" s="4"/>
     </row>
-    <row r="125" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C125">
@@ -9421,7 +9364,7 @@
       <c r="S125" s="4"/>
       <c r="T125" s="4"/>
     </row>
-    <row r="126" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>387</v>
       </c>
@@ -9527,7 +9470,7 @@
       <c r="S127" s="4"/>
       <c r="T127" s="4"/>
     </row>
-    <row r="128" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>393</v>
       </c>
@@ -9578,10 +9521,12 @@
       <c r="R128" t="s">
         <v>395</v>
       </c>
-      <c r="S128" s="4"/>
+      <c r="S128" s="4" t="s">
+        <v>450</v>
+      </c>
       <c r="T128" s="4"/>
     </row>
-    <row r="129" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>396</v>
       </c>
@@ -9635,7 +9580,7 @@
       <c r="S129" s="4"/>
       <c r="T129" s="4"/>
     </row>
-    <row r="130" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>399</v>
       </c>
@@ -9689,7 +9634,7 @@
       <c r="S130" s="4"/>
       <c r="T130" s="4"/>
     </row>
-    <row r="131" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>402</v>
       </c>
@@ -9798,7 +9743,7 @@
       <c r="S132" s="4"/>
       <c r="T132" s="4"/>
     </row>
-    <row r="133" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>408</v>
       </c>
@@ -10119,7 +10064,7 @@
       <c r="S138" s="4"/>
       <c r="T138" s="4"/>
     </row>
-    <row r="139" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>426</v>
       </c>
@@ -10173,7 +10118,7 @@
       <c r="S139" s="4"/>
       <c r="T139" s="4"/>
     </row>
-    <row r="140" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>429</v>
       </c>
@@ -10227,7 +10172,7 @@
       <c r="S140" s="4"/>
       <c r="T140" s="4"/>
     </row>
-    <row r="141" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>432</v>
       </c>
@@ -10282,7 +10227,7 @@
       <c r="S141" s="4"/>
       <c r="T141" s="4"/>
     </row>
-    <row r="142" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" ht="15" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
         <v>434</v>
       </c>
@@ -10331,10 +10276,12 @@
       <c r="R142" t="s">
         <v>251</v>
       </c>
-      <c r="S142" s="4"/>
+      <c r="S142" s="4" t="s">
+        <v>449</v>
+      </c>
       <c r="T142" s="4"/>
     </row>
-    <row r="143" spans="1:20" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20" ht="15" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="9" t="s">
         <v>436</v>
       </c>
@@ -10386,11 +10333,11 @@
       <c r="S143" s="4"/>
       <c r="T143" s="4"/>
     </row>
-    <row r="144" spans="1:20" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C144">
@@ -10439,7 +10386,7 @@
       <c r="S144" s="4"/>
       <c r="T144" s="4"/>
     </row>
-    <row r="145" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>441</v>
       </c>
@@ -10490,7 +10437,7 @@
       <c r="S145" s="4"/>
       <c r="T145" s="4"/>
     </row>
-    <row r="146" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
         <v>444</v>
       </c>
@@ -10544,734 +10491,733 @@
   </sheetData>
   <autoFilter ref="A1:T146" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="11">
-      <filters blank="1"/>
-    </filterColumn>
-    <filterColumn colId="15">
-      <colorFilter dxfId="1" cellColor="0"/>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="P2:P146">
-    <cfRule type="cellIs" dxfId="149" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="145" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="cellIs" dxfId="148" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="144" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="cellIs" dxfId="147" priority="5" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="143" priority="5" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="cellIs" dxfId="146" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="142" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="cellIs" dxfId="145" priority="9" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="141" priority="9" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6">
-    <cfRule type="cellIs" dxfId="144" priority="11" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="140" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="cellIs" dxfId="143" priority="13" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="139" priority="13" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8">
-    <cfRule type="cellIs" dxfId="142" priority="15" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="138" priority="15" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="cellIs" dxfId="141" priority="17" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="137" priority="17" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O10">
-    <cfRule type="cellIs" dxfId="140" priority="19" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="136" priority="19" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="cellIs" dxfId="139" priority="21" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="135" priority="21" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12">
-    <cfRule type="cellIs" dxfId="138" priority="23" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="134" priority="23" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O13">
-    <cfRule type="cellIs" dxfId="137" priority="25" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="133" priority="25" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O14">
-    <cfRule type="cellIs" dxfId="136" priority="27" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="132" priority="27" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15">
-    <cfRule type="cellIs" dxfId="135" priority="29" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="131" priority="29" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O16">
-    <cfRule type="cellIs" dxfId="134" priority="31" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="130" priority="31" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17">
-    <cfRule type="cellIs" dxfId="133" priority="33" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="129" priority="33" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O18">
-    <cfRule type="cellIs" dxfId="132" priority="35" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="128" priority="35" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O19">
-    <cfRule type="cellIs" dxfId="131" priority="37" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="127" priority="37" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O20">
-    <cfRule type="cellIs" dxfId="130" priority="39" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="126" priority="39" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O21">
-    <cfRule type="cellIs" dxfId="129" priority="41" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="125" priority="41" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O22">
-    <cfRule type="cellIs" dxfId="128" priority="43" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="124" priority="43" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23">
-    <cfRule type="cellIs" dxfId="127" priority="45" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="123" priority="45" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O24">
-    <cfRule type="cellIs" dxfId="126" priority="47" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="122" priority="47" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O25">
-    <cfRule type="cellIs" dxfId="125" priority="49" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="121" priority="49" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O26">
-    <cfRule type="cellIs" dxfId="124" priority="51" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="120" priority="51" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O27">
-    <cfRule type="cellIs" dxfId="123" priority="53" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="119" priority="53" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O28">
-    <cfRule type="cellIs" dxfId="122" priority="55" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="55" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O29">
-    <cfRule type="cellIs" dxfId="121" priority="57" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="117" priority="57" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O30">
-    <cfRule type="cellIs" dxfId="120" priority="59" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="116" priority="59" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O31">
-    <cfRule type="cellIs" dxfId="119" priority="61" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="115" priority="61" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O32">
-    <cfRule type="cellIs" dxfId="118" priority="63" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="114" priority="63" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O33">
-    <cfRule type="cellIs" dxfId="117" priority="65" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="65" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O34">
-    <cfRule type="cellIs" dxfId="116" priority="67" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="112" priority="67" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O35">
-    <cfRule type="cellIs" dxfId="115" priority="69" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="111" priority="69" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="cellIs" dxfId="114" priority="71" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="110" priority="71" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O37">
-    <cfRule type="cellIs" dxfId="113" priority="73" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="109" priority="73" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O38">
-    <cfRule type="cellIs" dxfId="112" priority="75" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="108" priority="75" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O39">
-    <cfRule type="cellIs" dxfId="111" priority="77" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="107" priority="77" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O40">
-    <cfRule type="cellIs" dxfId="110" priority="79" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="79" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O41">
-    <cfRule type="cellIs" dxfId="109" priority="81" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="105" priority="81" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O42">
-    <cfRule type="cellIs" dxfId="108" priority="83" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="104" priority="83" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O43">
-    <cfRule type="cellIs" dxfId="107" priority="85" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="85" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O44">
-    <cfRule type="cellIs" dxfId="106" priority="87" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="87" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O45">
-    <cfRule type="cellIs" dxfId="105" priority="89" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="101" priority="89" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O46">
-    <cfRule type="cellIs" dxfId="104" priority="91" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="91" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O47">
-    <cfRule type="cellIs" dxfId="103" priority="93" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="99" priority="93" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O48">
-    <cfRule type="cellIs" dxfId="102" priority="95" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="98" priority="95" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49">
-    <cfRule type="cellIs" dxfId="101" priority="97" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="97" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O50">
-    <cfRule type="cellIs" dxfId="100" priority="99" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="99" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O51">
-    <cfRule type="cellIs" dxfId="99" priority="101" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="101" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O52">
-    <cfRule type="cellIs" dxfId="98" priority="103" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="103" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O53">
-    <cfRule type="cellIs" dxfId="97" priority="105" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="93" priority="105" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54">
-    <cfRule type="cellIs" dxfId="96" priority="107" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="92" priority="107" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O55">
-    <cfRule type="cellIs" dxfId="95" priority="109" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="109" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O56">
-    <cfRule type="cellIs" dxfId="94" priority="111" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="90" priority="111" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O57">
-    <cfRule type="cellIs" dxfId="93" priority="113" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="89" priority="113" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O58">
-    <cfRule type="cellIs" dxfId="92" priority="115" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="115" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O59">
-    <cfRule type="cellIs" dxfId="91" priority="117" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="117" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O60">
-    <cfRule type="cellIs" dxfId="90" priority="119" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="119" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O61">
-    <cfRule type="cellIs" dxfId="89" priority="121" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="121" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O62">
-    <cfRule type="cellIs" dxfId="88" priority="123" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="123" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O63">
-    <cfRule type="cellIs" dxfId="87" priority="125" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="125" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O64">
-    <cfRule type="cellIs" dxfId="86" priority="127" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="127" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O65">
-    <cfRule type="cellIs" dxfId="85" priority="129" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="129" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O66">
-    <cfRule type="cellIs" dxfId="84" priority="131" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="80" priority="131" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O67">
-    <cfRule type="cellIs" dxfId="83" priority="133" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="133" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O68">
-    <cfRule type="cellIs" dxfId="82" priority="135" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="135" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O69">
-    <cfRule type="cellIs" dxfId="81" priority="137" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="137" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O70">
-    <cfRule type="cellIs" dxfId="80" priority="139" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="139" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O71">
-    <cfRule type="cellIs" dxfId="79" priority="141" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="141" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O72">
-    <cfRule type="cellIs" dxfId="78" priority="143" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="143" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73">
-    <cfRule type="cellIs" dxfId="77" priority="145" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="145" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O74">
-    <cfRule type="cellIs" dxfId="76" priority="147" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="147" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O75">
-    <cfRule type="cellIs" dxfId="75" priority="149" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="149" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O76">
-    <cfRule type="cellIs" dxfId="74" priority="151" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="151" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O77">
-    <cfRule type="cellIs" dxfId="73" priority="153" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="153" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O78">
-    <cfRule type="cellIs" dxfId="72" priority="155" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="155" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O79">
-    <cfRule type="cellIs" dxfId="71" priority="157" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="157" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O80">
-    <cfRule type="cellIs" dxfId="70" priority="159" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="159" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O81">
-    <cfRule type="cellIs" dxfId="69" priority="161" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="161" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O82">
-    <cfRule type="cellIs" dxfId="68" priority="163" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="163" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O83">
-    <cfRule type="cellIs" dxfId="67" priority="165" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="165" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O84">
-    <cfRule type="cellIs" dxfId="66" priority="167" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="167" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O85">
-    <cfRule type="cellIs" dxfId="65" priority="169" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="169" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O86">
-    <cfRule type="cellIs" dxfId="64" priority="171" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="171" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O87">
-    <cfRule type="cellIs" dxfId="63" priority="173" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="173" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O88">
-    <cfRule type="cellIs" dxfId="62" priority="175" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="175" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O89">
-    <cfRule type="cellIs" dxfId="61" priority="177" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="177" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O90">
-    <cfRule type="cellIs" dxfId="60" priority="179" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="179" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O91">
-    <cfRule type="cellIs" dxfId="59" priority="181" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="181" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O92">
-    <cfRule type="cellIs" dxfId="58" priority="183" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="54" priority="183" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O93">
-    <cfRule type="cellIs" dxfId="57" priority="185" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="185" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94">
-    <cfRule type="cellIs" dxfId="56" priority="187" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="187" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O95">
-    <cfRule type="cellIs" dxfId="55" priority="189" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="189" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O96">
-    <cfRule type="cellIs" dxfId="54" priority="191" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="191" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O97">
-    <cfRule type="cellIs" dxfId="53" priority="193" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="193" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O99">
-    <cfRule type="cellIs" dxfId="51" priority="197" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="197" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O100">
-    <cfRule type="cellIs" dxfId="50" priority="199" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="199" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O101">
-    <cfRule type="cellIs" dxfId="49" priority="201" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="201" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O102">
-    <cfRule type="cellIs" dxfId="48" priority="203" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="203" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O103">
-    <cfRule type="cellIs" dxfId="47" priority="205" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="205" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O104">
-    <cfRule type="cellIs" dxfId="46" priority="207" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="207" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O105">
-    <cfRule type="cellIs" dxfId="45" priority="209" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="209" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O106">
-    <cfRule type="cellIs" dxfId="44" priority="211" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="211" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O107">
-    <cfRule type="cellIs" dxfId="43" priority="213" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="213" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O108">
-    <cfRule type="cellIs" dxfId="42" priority="215" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="215" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O109">
-    <cfRule type="cellIs" dxfId="41" priority="217" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="217" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O110">
-    <cfRule type="cellIs" dxfId="40" priority="219" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="219" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O111">
-    <cfRule type="cellIs" dxfId="39" priority="221" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="221" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O112">
-    <cfRule type="cellIs" dxfId="38" priority="223" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="223" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O113">
-    <cfRule type="cellIs" dxfId="37" priority="225" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="225" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O114">
-    <cfRule type="cellIs" dxfId="36" priority="227" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="227" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O115">
-    <cfRule type="cellIs" dxfId="35" priority="229" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="229" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O116">
-    <cfRule type="cellIs" dxfId="34" priority="231" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="231" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O117">
-    <cfRule type="cellIs" dxfId="33" priority="233" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="233" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O118">
-    <cfRule type="cellIs" dxfId="32" priority="235" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="235" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O119">
-    <cfRule type="cellIs" dxfId="31" priority="237" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="237" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O120">
-    <cfRule type="cellIs" dxfId="30" priority="239" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="239" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O121">
-    <cfRule type="cellIs" dxfId="29" priority="241" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="241" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O122">
-    <cfRule type="cellIs" dxfId="28" priority="243" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="243" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O123">
-    <cfRule type="cellIs" dxfId="27" priority="245" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="245" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O124">
-    <cfRule type="cellIs" dxfId="26" priority="247" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="247" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O125">
-    <cfRule type="cellIs" dxfId="25" priority="249" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="249" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O126">
-    <cfRule type="cellIs" dxfId="24" priority="251" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="251" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O127">
-    <cfRule type="cellIs" dxfId="23" priority="253" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="253" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O128">
-    <cfRule type="cellIs" dxfId="22" priority="255" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="255" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O129">
-    <cfRule type="cellIs" dxfId="21" priority="257" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="257" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O130">
-    <cfRule type="cellIs" dxfId="20" priority="259" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="259" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O131">
-    <cfRule type="cellIs" dxfId="19" priority="261" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="261" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O132">
-    <cfRule type="cellIs" dxfId="18" priority="263" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="263" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O133">
-    <cfRule type="cellIs" dxfId="17" priority="265" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="265" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O134">
-    <cfRule type="cellIs" dxfId="16" priority="267" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="267" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O135">
-    <cfRule type="cellIs" dxfId="15" priority="269" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="269" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O136">
-    <cfRule type="cellIs" dxfId="14" priority="271" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="271" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O137">
-    <cfRule type="cellIs" dxfId="13" priority="273" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="273" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O138">
-    <cfRule type="cellIs" dxfId="12" priority="275" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="275" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O139">
-    <cfRule type="cellIs" dxfId="11" priority="277" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="277" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O140">
-    <cfRule type="cellIs" dxfId="10" priority="279" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="279" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O141">
-    <cfRule type="cellIs" dxfId="9" priority="281" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="281" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O142">
-    <cfRule type="cellIs" dxfId="8" priority="283" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="283" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O143">
-    <cfRule type="cellIs" dxfId="7" priority="285" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="285" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O144">
-    <cfRule type="cellIs" dxfId="6" priority="287" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="287" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O145">
-    <cfRule type="cellIs" dxfId="5" priority="289" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="289" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O146">
-    <cfRule type="cellIs" dxfId="4" priority="291" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="291" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>